<commit_message>
Update template servizi czrm
</commit_message>
<xml_diff>
--- a/Template Servizi CzRM.xlsx
+++ b/Template Servizi CzRM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b737355\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F53C25-AC85-4249-A95A-6091A2B67019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEDB559-8FA2-4FEC-87D4-B5AD0A591A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Telefono</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Titolo card di contatto</t>
+  </si>
+  <si>
+    <t>Orario al pubblico del telefono</t>
+  </si>
+  <si>
+    <t>Link</t>
   </si>
 </sst>
 </file>
@@ -361,18 +367,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -380,10 +387,16 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>